<commit_message>
Update to initial requirements and design documentation
</commit_message>
<xml_diff>
--- a/requirements/mayhap_reqs.xlsx
+++ b/requirements/mayhap_reqs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="230">
   <si>
     <t>Theme</t>
   </si>
@@ -361,270 +361,378 @@
 Per project</t>
   </si>
   <si>
-    <t>Risk ID
+    <t>Set of risk event drivers</t>
+  </si>
+  <si>
+    <t>Set of impact drivers</t>
+  </si>
+  <si>
+    <t>Estimated total loss (Lt)</t>
+  </si>
+  <si>
+    <t>Expression of loss setting
+Loss units setting</t>
+  </si>
+  <si>
+    <t>Tool top-level
+(Per project?)</t>
+  </si>
+  <si>
+    <t>Expression of probability setting</t>
+  </si>
+  <si>
+    <t>Probability of risk event (Pe)</t>
+  </si>
+  <si>
+    <t>Probability of impact (Pi)</t>
+  </si>
+  <si>
+    <t>Expected loss (Le)</t>
+  </si>
+  <si>
+    <t>Maximum tolerated loss setting</t>
+  </si>
+  <si>
+    <t>Indication that decision made on risks to be managed</t>
+  </si>
+  <si>
+    <t>"</t>
+  </si>
+  <si>
+    <t>Risk priority</t>
+  </si>
+  <si>
+    <t>Maximum number of active risks setting</t>
+  </si>
+  <si>
+    <t>Risk owner
+Action plan owner</t>
+  </si>
+  <si>
+    <t>Per risk
+Per action plan</t>
+  </si>
+  <si>
+    <t>Set of risk planning decisions</t>
+  </si>
+  <si>
+    <t>Per action plan</t>
+  </si>
+  <si>
+    <t>Risk action plan type</t>
+  </si>
+  <si>
+    <t>Action plan trigger (Set? May be more than one trigger...)</t>
+  </si>
+  <si>
+    <t>Risk event driver reference</t>
+  </si>
+  <si>
+    <t>Impact driver reference</t>
+  </si>
+  <si>
+    <t>Per prevention action plan</t>
+  </si>
+  <si>
+    <t>Per contingency action plan</t>
+  </si>
+  <si>
+    <t>Estimated change in Pe</t>
+  </si>
+  <si>
+    <t>Estimated change in Pi
+Estimated change in Lt</t>
+  </si>
+  <si>
+    <t>(As per RR3?)</t>
+  </si>
+  <si>
+    <t>Action plan status</t>
+  </si>
+  <si>
+    <t>RR15</t>
+  </si>
+  <si>
+    <t>As a PM, when an action plan has been completed, I want to record the actual time and resources expended on the action plan, so that we can later review the effectiveness of our risk management.</t>
+  </si>
+  <si>
+    <t>Actual change in Pe
+Actual change in Pi
+Actual change in Lt</t>
+  </si>
+  <si>
+    <t>Estimated time required
+Estimated resources required</t>
+  </si>
+  <si>
+    <t>Risk reduction leverage</t>
+  </si>
+  <si>
+    <t>Actual time spent
+Actual resources spent</t>
+  </si>
+  <si>
+    <t>Set of action plans
+Action plan description</t>
+  </si>
+  <si>
+    <t>Risk status (in terms of whether it will be managed). The valid states are: Active and Inactive.</t>
+  </si>
+  <si>
+    <t>As a risk tool user, I want to identify risks that have been closed and risks that have become issues.</t>
+  </si>
+  <si>
+    <t>This requirement adds additional states to the Risk status field. These states are Issue and Closed.</t>
+  </si>
+  <si>
+    <t>MR2</t>
+  </si>
+  <si>
+    <t>As a risk tool user, I want to mark an active risk as an issue if the risk event still occurs in spite of prevention plans that have been put in place, so as to adhere to S&amp;M's process.</t>
+  </si>
+  <si>
+    <t>MR3</t>
+  </si>
+  <si>
+    <t>As a risk tool user, when a risk is marked as an issue, I want to explicitly identify the event driver that resulted in the risk event occurring, so that this information can be used in future.</t>
+  </si>
+  <si>
+    <t>MR4</t>
+  </si>
+  <si>
+    <t>As a risk tool user, once a risk has been marked as an issue, I want the focus to be on the contingency plans that aim to mitigate the total loss.</t>
+  </si>
+  <si>
+    <t>MR5</t>
+  </si>
+  <si>
+    <t>As a risk tool user, I want to mark an active risk as closed if the risk event was successfully prevented from occurring.</t>
+  </si>
+  <si>
+    <t>MR6</t>
+  </si>
+  <si>
+    <t>As a risk tool user, I want to mark an active risk as closed if the time component or condition of the risk event has passed and the event did not occur.</t>
+  </si>
+  <si>
+    <t>MR7</t>
+  </si>
+  <si>
+    <t>As a risk tool user, I want to mark an active risk as closed if the risk became an issue and we have finished managing the issue via contingency plans.</t>
+  </si>
+  <si>
+    <t>Risk status. The valid states are: Active, Inactive, Issue, Closed.</t>
+  </si>
+  <si>
+    <t>Risk event cause</t>
+  </si>
+  <si>
+    <t>Per issue</t>
+  </si>
+  <si>
+    <t>MR8</t>
+  </si>
+  <si>
+    <t>MR9</t>
+  </si>
+  <si>
+    <t>S&amp;M has some examples of graphical displays: Movement of risks on the risk map; Bar charts tracking expected loss over time.</t>
+  </si>
+  <si>
+    <t>As a PM, I want to record the status of each plan for each risk at our progress or review meetings, so that I can track the progress on the plans.</t>
+  </si>
+  <si>
+    <t>MR10</t>
+  </si>
+  <si>
+    <t>As a PM, I want the risk tool to provide a checklist of things to review in team meetings, so that I don't forget to review key things, and so that the team gets used to a risk review process.</t>
+  </si>
+  <si>
+    <t>E.g., the process on page 132 of S&amp;M.</t>
+  </si>
+  <si>
+    <t>MR11</t>
+  </si>
+  <si>
+    <t>MR12</t>
+  </si>
+  <si>
+    <t>This is one of the strategic metrics recommended by S&amp;M.</t>
+  </si>
+  <si>
+    <t>MR13</t>
+  </si>
+  <si>
+    <t>As a PM, I want a graphical representation of risk status trend, i.e., the number of risks in the Active, Closed and Issue statuses per monitoring period, so that I can track and communicate risks.</t>
+  </si>
+  <si>
+    <t>MR14</t>
+  </si>
+  <si>
+    <t>As a PM, I want a graphical representation of the status of the current risks, so that I can track and communicate risks.</t>
+  </si>
+  <si>
+    <t>MR15</t>
+  </si>
+  <si>
+    <t>As a PM, I want a graphical representation of the total, expected and actual losses of all risks per monitoring period, so that I can track and communicate risks.</t>
+  </si>
+  <si>
+    <t>MR16</t>
+  </si>
+  <si>
+    <t>As a PM, I want a graphical representation of the losses of the active and inactive risks, so that I can track and communicate risks.</t>
+  </si>
+  <si>
+    <t>This is one of the tactical metrics recommended by S&amp;M.</t>
+  </si>
+  <si>
+    <t>MR17</t>
+  </si>
+  <si>
+    <t>As a PM, I want key metrics to be available on a dashboard, so that I can easily see and communicate risk status and trends.</t>
+  </si>
+  <si>
+    <t>Although the Risk ID is listed here as a field to be captured, it should actually be generated automatically by the risk tool. Risk IDs should be unique within the "project".
+Isn't it a bit early in the process to identify a risk owner? Prioritization hasn't happened yet, so the risk might not even be managed. Maybe what should be captured here is the risk originator.</t>
+  </si>
+  <si>
+    <t>The same scale used for the risk event probability should be used, with the addition of a 100% option. "It is entirely possible for the probability of the impact to be a certainty."</t>
+  </si>
+  <si>
+    <t>Risks that will be managed should have the status Active, and risks that will not be managed should have the status Inactive.</t>
+  </si>
+  <si>
+    <t>As a PM, I want to indicate to the tool any additional risks that will be managed, regardless of their position on the risk map.</t>
+  </si>
+  <si>
+    <t>As a PM, I want to indicate to the tool any additional risks that will not be managed, regardless of their position on the risk map.</t>
+  </si>
+  <si>
+    <t>As a PM, I want to configure the number of risks that will be managed and have the risk tool warn me when I have exceeded this value, so that I am conscious of using too many resources for risk management.</t>
+  </si>
+  <si>
+    <t>As a PM, I want a graphical display of how well we are progressing in managing the projects risks overall, so that the overall status can be quickly reviewed in team meetings, and reported to other stakeholders.</t>
+  </si>
+  <si>
+    <t>As a PM, I want the tool to record per project the number of risks identified and averted due to risk management, so that I can track and communicate the effectiveness of our risk management program.</t>
+  </si>
+  <si>
+    <t>As a PM, I want the tool to record per project the number of risks that went unidentified and later occurred, so that I can track and communicate the effectiveness of our risk management program.</t>
+  </si>
+  <si>
+    <t>Risk ID (or name)
 Risk originator
 Risk event description
 Impact description</t>
   </si>
   <si>
-    <t>Set of risk event drivers</t>
-  </si>
-  <si>
-    <t>Set of impact drivers</t>
-  </si>
-  <si>
-    <t>Estimated total loss (Lt)</t>
-  </si>
-  <si>
-    <t>Expression of loss setting
-Loss units setting</t>
-  </si>
-  <si>
-    <t>Tool top-level
-(Per project?)</t>
-  </si>
-  <si>
-    <t>Expression of probability setting</t>
-  </si>
-  <si>
-    <t>Probability of risk event (Pe)</t>
-  </si>
-  <si>
-    <t>Probability of impact (Pi)</t>
-  </si>
-  <si>
-    <t>Expected loss (Le)</t>
-  </si>
-  <si>
-    <t>Maximum tolerated loss setting</t>
-  </si>
-  <si>
-    <t>Indication that decision made on risks to be managed</t>
-  </si>
-  <si>
-    <t>"</t>
-  </si>
-  <si>
-    <t>Risk priority</t>
-  </si>
-  <si>
-    <t>Maximum number of active risks setting</t>
-  </si>
-  <si>
-    <t>Risk owner
-Action plan owner</t>
-  </si>
-  <si>
-    <t>Per risk
-Per action plan</t>
-  </si>
-  <si>
-    <t>Set of risk planning decisions</t>
-  </si>
-  <si>
-    <t>Per action plan</t>
-  </si>
-  <si>
-    <t>Risk action plan type</t>
-  </si>
-  <si>
-    <t>Action plan trigger (Set? May be more than one trigger...)</t>
-  </si>
-  <si>
-    <t>Risk event driver reference</t>
-  </si>
-  <si>
-    <t>Impact driver reference</t>
-  </si>
-  <si>
-    <t>Per prevention action plan</t>
-  </si>
-  <si>
-    <t>Per contingency action plan</t>
-  </si>
-  <si>
-    <t>Estimated change in Pe</t>
-  </si>
-  <si>
-    <t>Estimated change in Pi
-Estimated change in Lt</t>
-  </si>
-  <si>
-    <t>(As per RR3?)</t>
-  </si>
-  <si>
-    <t>Action plan status</t>
-  </si>
-  <si>
-    <t>RR15</t>
-  </si>
-  <si>
-    <t>As a PM, when an action plan has been completed, I want to record the actual time and resources expended on the action plan, so that we can later review the effectiveness of our risk management.</t>
-  </si>
-  <si>
-    <t>Actual change in Pe
-Actual change in Pi
-Actual change in Lt</t>
-  </si>
-  <si>
-    <t>Estimated time required
-Estimated resources required</t>
-  </si>
-  <si>
-    <t>Risk reduction leverage</t>
-  </si>
-  <si>
-    <t>Actual time spent
-Actual resources spent</t>
-  </si>
-  <si>
-    <t>Set of action plans
-Action plan description</t>
-  </si>
-  <si>
-    <t>Risk status (in terms of whether it will be managed). The valid states are: Active and Inactive.</t>
-  </si>
-  <si>
-    <t>As a risk tool user, I want to identify risks that have been closed and risks that have become issues.</t>
-  </si>
-  <si>
-    <t>This requirement adds additional states to the Risk status field. These states are Issue and Closed.</t>
-  </si>
-  <si>
-    <t>MR2</t>
-  </si>
-  <si>
-    <t>As a risk tool user, I want to mark an active risk as an issue if the risk event still occurs in spite of prevention plans that have been put in place, so as to adhere to S&amp;M's process.</t>
-  </si>
-  <si>
-    <t>MR3</t>
-  </si>
-  <si>
-    <t>As a risk tool user, when a risk is marked as an issue, I want to explicitly identify the event driver that resulted in the risk event occurring, so that this information can be used in future.</t>
-  </si>
-  <si>
-    <t>MR4</t>
-  </si>
-  <si>
-    <t>As a risk tool user, once a risk has been marked as an issue, I want the focus to be on the contingency plans that aim to mitigate the total loss.</t>
-  </si>
-  <si>
-    <t>MR5</t>
-  </si>
-  <si>
-    <t>As a risk tool user, I want to mark an active risk as closed if the risk event was successfully prevented from occurring.</t>
-  </si>
-  <si>
-    <t>MR6</t>
-  </si>
-  <si>
-    <t>As a risk tool user, I want to mark an active risk as closed if the time component or condition of the risk event has passed and the event did not occur.</t>
-  </si>
-  <si>
-    <t>MR7</t>
-  </si>
-  <si>
-    <t>As a risk tool user, I want to mark an active risk as closed if the risk became an issue and we have finished managing the issue via contingency plans.</t>
-  </si>
-  <si>
-    <t>Risk status. The valid states are: Active, Inactive, Issue, Closed.</t>
-  </si>
-  <si>
-    <t>Risk event cause</t>
-  </si>
-  <si>
-    <t>Per issue</t>
-  </si>
-  <si>
-    <t>MR8</t>
-  </si>
-  <si>
-    <t>MR9</t>
-  </si>
-  <si>
-    <t>S&amp;M has some examples of graphical displays: Movement of risks on the risk map; Bar charts tracking expected loss over time.</t>
-  </si>
-  <si>
-    <t>As a PM, I want to record the status of each plan for each risk at our progress or review meetings, so that I can track the progress on the plans.</t>
-  </si>
-  <si>
-    <t>MR10</t>
-  </si>
-  <si>
-    <t>As a PM, I want the risk tool to provide a checklist of things to review in team meetings, so that I don't forget to review key things, and so that the team gets used to a risk review process.</t>
-  </si>
-  <si>
-    <t>E.g., the process on page 132 of S&amp;M.</t>
-  </si>
-  <si>
-    <t>MR11</t>
-  </si>
-  <si>
-    <t>MR12</t>
-  </si>
-  <si>
-    <t>This is one of the strategic metrics recommended by S&amp;M.</t>
-  </si>
-  <si>
-    <t>MR13</t>
-  </si>
-  <si>
-    <t>As a PM, I want a graphical representation of risk status trend, i.e., the number of risks in the Active, Closed and Issue statuses per monitoring period, so that I can track and communicate risks.</t>
-  </si>
-  <si>
-    <t>MR14</t>
-  </si>
-  <si>
-    <t>As a PM, I want a graphical representation of the status of the current risks, so that I can track and communicate risks.</t>
-  </si>
-  <si>
-    <t>MR15</t>
-  </si>
-  <si>
-    <t>As a PM, I want a graphical representation of the total, expected and actual losses of all risks per monitoring period, so that I can track and communicate risks.</t>
-  </si>
-  <si>
-    <t>MR16</t>
-  </si>
-  <si>
-    <t>As a PM, I want a graphical representation of the losses of the active and inactive risks, so that I can track and communicate risks.</t>
-  </si>
-  <si>
-    <t>This is one of the tactical metrics recommended by S&amp;M.</t>
-  </si>
-  <si>
-    <t>MR17</t>
-  </si>
-  <si>
-    <t>As a PM, I want key metrics to be available on a dashboard, so that I can easily see and communicate risk status and trends.</t>
-  </si>
-  <si>
-    <t>Although the Risk ID is listed here as a field to be captured, it should actually be generated automatically by the risk tool. Risk IDs should be unique within the "project".
-Isn't it a bit early in the process to identify a risk owner? Prioritization hasn't happened yet, so the risk might not even be managed. Maybe what should be captured here is the risk originator.</t>
-  </si>
-  <si>
-    <t>The same scale used for the risk event probability should be used, with the addition of a 100% option. "It is entirely possible for the probability of the impact to be a certainty."</t>
-  </si>
-  <si>
-    <t>Risks that will be managed should have the status Active, and risks that will not be managed should have the status Inactive.</t>
-  </si>
-  <si>
-    <t>As a PM, I want to indicate to the tool any additional risks that will be managed, regardless of their position on the risk map.</t>
-  </si>
-  <si>
-    <t>As a PM, I want to indicate to the tool any additional risks that will not be managed, regardless of their position on the risk map.</t>
-  </si>
-  <si>
-    <t>As a PM, I want to configure the number of risks that will be managed and have the risk tool warn me when I have exceeded this value, so that I am conscious of using too many resources for risk management.</t>
-  </si>
-  <si>
-    <t>As a PM, I want a graphical display of how well we are progressing in managing the projects risks overall, so that the overall status can be quickly reviewed in team meetings, and reported to other stakeholders.</t>
-  </si>
-  <si>
-    <t>As a PM, I want the tool to record per project the number of risks identified and averted due to risk management, so that I can track and communicate the effectiveness of our risk management program.</t>
-  </si>
-  <si>
-    <t>As a PM, I want the tool to record per project the number of risks that went unidentified and later occurred, so that I can track and communicate the effectiveness of our risk management program.</t>
+    <t>Associated Data Element</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Calculate when risk accessed.</t>
+  </si>
+  <si>
+    <t>risk</t>
+  </si>
+  <si>
+    <t>discovery_approach</t>
+  </si>
+  <si>
+    <t>Database Field(s)</t>
+  </si>
+  <si>
+    <t>name
+originator
+event_description
+impact_description</t>
+  </si>
+  <si>
+    <t>Database Table(s)</t>
+  </si>
+  <si>
+    <t>project
+risk</t>
+  </si>
+  <si>
+    <t>Get project risks by querying risk table by project_id.</t>
+  </si>
+  <si>
+    <t>event_driver</t>
+  </si>
+  <si>
+    <t>Get event drivers by querying event_driver table by risk_id.</t>
+  </si>
+  <si>
+    <t>impact_driver</t>
+  </si>
+  <si>
+    <t>Get impact drivers by querying impact_driver table by risk_id.</t>
+  </si>
+  <si>
+    <t>estimated_total_loss</t>
+  </si>
+  <si>
+    <t>project</t>
+  </si>
+  <si>
+    <t>loss_type
+loss_units</t>
+  </si>
+  <si>
+    <t>probability_setting</t>
+  </si>
+  <si>
+    <t>event_probability</t>
+  </si>
+  <si>
+    <t>impact_probability</t>
+  </si>
+  <si>
+    <t>expected_loss</t>
+  </si>
+  <si>
+    <t>maximum_loss</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>priority</t>
+  </si>
+  <si>
+    <t>maximum_risks</t>
+  </si>
+  <si>
+    <t>plan</t>
+  </si>
+  <si>
+    <t>owner</t>
+  </si>
+  <si>
+    <t>plan
+risk_plan</t>
+  </si>
+  <si>
+    <t>Get risk action plans by querying risk_plan table by risk_id.</t>
+  </si>
+  <si>
+    <t>IR4</t>
+  </si>
+  <si>
+    <t>Identifying risks should be quick and easy, i.e., compatible with a brainstorming session.</t>
+  </si>
+  <si>
+    <t>Capture an event, capture its impact, move on. All of this happens quickly. The group can't be left waiting for the facilitator to open another risk or save the risk, etc.</t>
   </si>
 </sst>
 </file>
@@ -1030,10 +1138,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L65"/>
+  <dimension ref="A1:L66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1044,6 +1152,9 @@
     <col min="4" max="4" width="50.7109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="52.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -1063,6 +1174,18 @@
       <c r="F1" s="5" t="s">
         <v>106</v>
       </c>
+      <c r="G1" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="2" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -1083,6 +1206,12 @@
       </c>
       <c r="G2" s="1" t="s">
         <v>111</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="45" x14ac:dyDescent="0.25">
@@ -1111,7 +1240,7 @@
         <v>104</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="45" x14ac:dyDescent="0.25">
@@ -1128,6 +1257,12 @@
       </c>
       <c r="G5" t="s">
         <v>109</v>
+      </c>
+      <c r="H5" t="s">
+        <v>197</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1140,7 +1275,7 @@
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
       <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
+      <c r="J6" s="10"/>
       <c r="K6" s="8"/>
       <c r="L6" s="8"/>
     </row>
@@ -1164,6 +1299,12 @@
       <c r="G7" t="s">
         <v>109</v>
       </c>
+      <c r="H7" t="s">
+        <v>200</v>
+      </c>
+      <c r="I7" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="8" spans="1:12" ht="120" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="s">
@@ -1173,14 +1314,20 @@
         <v>19</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E8" s="8"/>
       <c r="F8" s="1" t="s">
-        <v>112</v>
+        <v>195</v>
       </c>
       <c r="G8" t="s">
         <v>109</v>
+      </c>
+      <c r="H8" t="s">
+        <v>200</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="45" x14ac:dyDescent="0.25">
@@ -1192,518 +1339,605 @@
       </c>
       <c r="E9" s="8"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
+    <row r="10" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="B10" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>229</v>
+      </c>
       <c r="E10" s="8"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
-    </row>
-    <row r="11" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="8"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+    </row>
+    <row r="12" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B12" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="G11" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="E12" s="8"/>
       <c r="F12" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G12" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="H12" t="s">
+        <v>207</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" s="2"/>
+        <v>29</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="E13" s="8"/>
       <c r="F13" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G13" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="H13" t="s">
+        <v>209</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="7" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>34</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="D14" s="2"/>
       <c r="E14" s="8"/>
       <c r="F14" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G14" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="H14" t="s">
+        <v>200</v>
+      </c>
+      <c r="I14" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D15" s="2"/>
+        <v>53</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="E15" s="8"/>
-    </row>
-    <row r="16" spans="1:12" ht="120" x14ac:dyDescent="0.25">
+      <c r="F15" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="G15" t="s">
+        <v>110</v>
+      </c>
+      <c r="H15" t="s">
+        <v>212</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>39</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="D16" s="2"/>
       <c r="E16" s="8"/>
-      <c r="F16" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="G16" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:12" ht="120" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E17" s="8"/>
       <c r="F17" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G17" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+      <c r="H17" t="s">
+        <v>212</v>
+      </c>
+      <c r="I17" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D18" s="2"/>
+        <v>38</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="E18" s="8"/>
-    </row>
-    <row r="19" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="F18" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="G18" t="s">
+        <v>109</v>
+      </c>
+      <c r="H18" t="s">
+        <v>200</v>
+      </c>
+      <c r="I18" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="7" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>188</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="D19" s="2"/>
       <c r="E19" s="8"/>
-      <c r="F19" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="G19" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D20" s="2"/>
+        <v>42</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>187</v>
+      </c>
       <c r="E20" s="8"/>
+      <c r="F20" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G20" t="s">
+        <v>109</v>
+      </c>
+      <c r="H20" t="s">
+        <v>200</v>
+      </c>
+      <c r="I20" t="s">
+        <v>216</v>
+      </c>
     </row>
     <row r="21" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>45</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="D21" s="2"/>
       <c r="E21" s="8"/>
-      <c r="F21" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="G21" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E22" s="8"/>
+      <c r="F22" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G22" t="s">
+        <v>109</v>
+      </c>
+      <c r="H22" t="s">
+        <v>200</v>
+      </c>
+      <c r="I22" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A23" s="3"/>
+      <c r="B23" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D22" s="2"/>
-      <c r="E22" s="8"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="12"/>
-      <c r="B23" s="9"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="11"/>
-      <c r="K23" s="11"/>
-      <c r="L23" s="11"/>
-    </row>
-    <row r="24" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+      <c r="D23" s="2"/>
+      <c r="E23" s="8"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="12"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="11"/>
+    </row>
+    <row r="25" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B25" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D25" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="E24" s="8"/>
-    </row>
-    <row r="25" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
-      <c r="B25" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="E25" s="8"/>
-      <c r="F25" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="G25" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="7" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>65</v>
       </c>
       <c r="E26" s="8"/>
-    </row>
-    <row r="27" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="F26" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="G26" t="s">
+        <v>110</v>
+      </c>
+      <c r="H26" t="s">
+        <v>212</v>
+      </c>
+      <c r="I26" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>189</v>
+        <v>67</v>
       </c>
       <c r="E27" s="8"/>
-      <c r="F27" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="G27" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>190</v>
+        <v>69</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>72</v>
+        <v>188</v>
       </c>
       <c r="E28" s="8"/>
       <c r="F28" s="1" t="s">
-        <v>148</v>
+        <v>122</v>
       </c>
       <c r="G28" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+      <c r="H28" t="s">
+        <v>219</v>
+      </c>
+      <c r="I28" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>72</v>
       </c>
       <c r="E29" s="8"/>
       <c r="F29" s="1" t="s">
-        <v>124</v>
+        <v>147</v>
       </c>
       <c r="G29" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="H29" t="s">
+        <v>200</v>
+      </c>
+      <c r="I29" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>73</v>
+        <v>190</v>
       </c>
       <c r="E30" s="8"/>
       <c r="F30" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G30" t="s">
-        <v>109</v>
+        <v>123</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="B31" s="7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E31" s="8"/>
       <c r="F31" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G31" t="s">
+        <v>109</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="3"/>
+      <c r="B32" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E32" s="8"/>
+      <c r="F32" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="G32" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="12"/>
-      <c r="B32" s="12"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="8"/>
-      <c r="F32" s="10"/>
-      <c r="G32" s="8"/>
-      <c r="H32" s="8"/>
-      <c r="I32" s="8"/>
-      <c r="J32" s="8"/>
-      <c r="K32" s="8"/>
-      <c r="L32" s="8"/>
-    </row>
-    <row r="33" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+      <c r="H32" t="s">
+        <v>212</v>
+      </c>
+      <c r="I32" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="12"/>
+      <c r="B33" s="12"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8"/>
+      <c r="J33" s="10"/>
+      <c r="K33" s="8"/>
+      <c r="L33" s="8"/>
+    </row>
+    <row r="34" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="B34" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C34" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="E33" s="8"/>
-      <c r="F33" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="3"/>
-      <c r="B34" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>78</v>
       </c>
       <c r="E34" s="8"/>
       <c r="F34" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="G34" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="G34" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="H34" s="1"/>
+    </row>
+    <row r="35" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
       <c r="B35" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E35" s="8"/>
       <c r="F35" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="G35" t="s">
-        <v>109</v>
+        <v>126</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="36" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E36" s="8"/>
       <c r="F36" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="G36" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E37" s="8"/>
       <c r="F37" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="G37" s="1" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="G37" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="7" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="E38" s="8"/>
       <c r="F38" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="G38" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
       <c r="B39" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>87</v>
+        <v>102</v>
       </c>
       <c r="E39" s="8"/>
       <c r="F39" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G39" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
       <c r="B40" s="7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E40" s="8"/>
       <c r="F40" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="G40" t="s">
         <v>134</v>
       </c>
-      <c r="G40" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
       <c r="B41" s="7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E41" s="8"/>
       <c r="F41" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="G41" t="s">
         <v>135</v>
@@ -1712,310 +1946,326 @@
     <row r="42" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
       <c r="B42" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E42" s="8"/>
       <c r="F42" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G42" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="43" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>
       <c r="B43" s="7" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E43" s="8"/>
       <c r="F43" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
+      </c>
+      <c r="G43" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="44" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
       <c r="B44" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E44" s="8"/>
       <c r="F44" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="G44" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
     </row>
     <row r="45" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
       <c r="B45" s="7" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D45" s="2"/>
+        <v>97</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>98</v>
+      </c>
       <c r="E45" s="8"/>
       <c r="F45" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G45" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
       <c r="B46" s="7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" s="8"/>
       <c r="F46" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="G46" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
       <c r="B47" s="7" t="s">
-        <v>141</v>
+        <v>101</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>142</v>
+        <v>103</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" s="8"/>
       <c r="F47" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G47" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A48" s="12"/>
-      <c r="B48" s="12"/>
-      <c r="C48" s="12"/>
-      <c r="D48" s="12"/>
+        <v>129</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A48" s="3"/>
+      <c r="B48" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D48" s="2"/>
       <c r="E48" s="8"/>
-      <c r="F48" s="10"/>
-      <c r="G48" s="8"/>
-      <c r="H48" s="8"/>
-      <c r="I48" s="8"/>
-      <c r="J48" s="8"/>
-      <c r="K48" s="8"/>
-      <c r="L48" s="8"/>
-    </row>
-    <row r="49" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
+      <c r="F48" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="G48" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A49" s="12"/>
+      <c r="B49" s="12"/>
+      <c r="C49" s="12"/>
+      <c r="D49" s="12"/>
+      <c r="E49" s="8"/>
+      <c r="F49" s="10"/>
+      <c r="G49" s="8"/>
+      <c r="H49" s="8"/>
+      <c r="I49" s="8"/>
+      <c r="J49" s="10"/>
+      <c r="K49" s="8"/>
+      <c r="L49" s="8"/>
+    </row>
+    <row r="50" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B49" s="7" t="s">
+      <c r="B50" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C50" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D50" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="D49" s="2" t="s">
+      <c r="E50" s="8"/>
+      <c r="F50" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="G50" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="B51" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="E49" s="8"/>
-      <c r="F49" s="1" t="s">
+      <c r="C51" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E51" s="8"/>
+    </row>
+    <row r="52" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="B52" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="E52" s="8"/>
+      <c r="F52" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="G49" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B50" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="E50" s="8"/>
-    </row>
-    <row r="51" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B51" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="C51" s="1" t="s">
+      <c r="G52" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="B53" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="E51" s="8"/>
-      <c r="F51" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="G51" s="1" t="s">
+      <c r="C53" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="E53" s="8"/>
+    </row>
+    <row r="54" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="B54" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E54" s="8"/>
+    </row>
+    <row r="55" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="B55" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E55" s="8"/>
+    </row>
+    <row r="56" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="B56" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E56" s="8"/>
+    </row>
+    <row r="57" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="B57" s="7" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B52" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="E52" s="8"/>
-    </row>
-    <row r="53" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B53" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="E53" s="8"/>
-    </row>
-    <row r="54" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B54" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="E54" s="8"/>
-    </row>
-    <row r="55" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B55" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="E55" s="8"/>
-    </row>
-    <row r="56" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B56" s="7" t="s">
+      <c r="C57" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="E57" s="8"/>
+    </row>
+    <row r="58" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="B58" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="C58" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E58" s="8"/>
+    </row>
+    <row r="59" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="B59" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="E59" s="8"/>
+    </row>
+    <row r="60" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="B60" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="C60" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="D56" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="E56" s="8"/>
-    </row>
-    <row r="57" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B57" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="E57" s="8"/>
-    </row>
-    <row r="58" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B58" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="E58" s="8"/>
-    </row>
-    <row r="59" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B59" s="7" t="s">
+      <c r="D60" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="E60" s="8"/>
+    </row>
+    <row r="61" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="B61" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="C61" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="D59" s="2" t="s">
+      <c r="D61" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="E61" s="8"/>
+    </row>
+    <row r="62" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="B62" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="E59" s="8"/>
-    </row>
-    <row r="60" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B60" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E60" s="8"/>
-    </row>
-    <row r="61" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B61" s="7" t="s">
+      <c r="C62" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="D62" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="E62" s="8"/>
+    </row>
+    <row r="63" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="B63" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="D61" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="E61" s="8"/>
-    </row>
-    <row r="62" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B62" s="7" t="s">
+      <c r="C63" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="C62" s="1" t="s">
+      <c r="D63" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="E63" s="8"/>
+    </row>
+    <row r="64" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="B64" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="D62" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="E62" s="8"/>
-    </row>
-    <row r="63" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B63" s="7" t="s">
+      <c r="C64" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="C63" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="D63" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="E63" s="8"/>
-    </row>
-    <row r="64" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B64" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="C64" s="1" t="s">
+      <c r="D64" s="2" t="s">
         <v>183</v>
-      </c>
-      <c r="D64" s="2" t="s">
-        <v>184</v>
       </c>
       <c r="E64" s="8"/>
     </row>
     <row r="65" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B65" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="E65" s="8"/>
+    </row>
+    <row r="66" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B66" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="C66" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="C65" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="E65" s="8"/>
+      <c r="E66" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>